<commit_message>
Aangegeven dat de visualisatiecodes voor de kleinere schalen niet op deze manier geïmplementeerd zijn.
</commit_message>
<xml_diff>
--- a/visualisatie/1.2.0/BRT_TOP10NL_1.2_visualisatiecode_attributen.xlsx
+++ b/visualisatie/1.2.0/BRT_TOP10NL_1.2_visualisatiecode_attributen.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BRT\BRT-datamodel\Visualisatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetkadaster-my.sharepoint.com/personal/daniel_tewinkel_kadaster_nl/Documents/_GITea_intern/dpigi-BRT-datamodel/Visualisatie/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_8E505039D5D4FDEB468762A140A06E5F424DA52D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB19A717-CF73-42DB-BF0B-9F159D20E4A0}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="180" windowWidth="20445" windowHeight="10650"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="13125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versie" sheetId="15" r:id="rId1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="350">
   <si>
     <t>type weg</t>
   </si>
@@ -1146,11 +1147,23 @@
   <si>
     <t>Datamodelwijziging februari 2019 verwerkt</t>
   </si>
+  <si>
+    <t>Tabblad visualisatie kleinschalige producten aangepast</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Actief</t>
+  </si>
+  <si>
+    <t>Niet geïmplementeerd</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1824,6 +1837,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1902,9 +1918,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1944,7 +1957,7 @@
     <cellStyle name="Notitie" xfId="35" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Ongeldig" xfId="36" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standaard_Objectcodes 2012-03" xfId="37"/>
+    <cellStyle name="Standaard_Objectcodes 2012-03" xfId="37" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="Titel" xfId="38" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Totaal" xfId="39" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Uitvoer" xfId="40" builtinId="21" customBuiltin="1"/>
@@ -2226,7 +2239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2236,14 +2249,14 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="46"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -2254,7 +2267,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="71">
+      <c r="A4" s="45">
         <v>41883</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2262,7 +2275,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="71">
+      <c r="A5" s="45">
         <v>42979</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2270,7 +2283,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="71">
+      <c r="A6" s="45">
         <v>43497</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2278,8 +2291,12 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="45">
+        <v>44832</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
@@ -2294,7 +2311,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2309,10 +2326,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="46"/>
     </row>
     <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
@@ -2436,7 +2453,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2450,10 +2467,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="46"/>
     </row>
     <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -2547,7 +2564,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2561,10 +2578,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="46"/>
     </row>
     <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
@@ -2768,7 +2785,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2782,10 +2799,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="46"/>
     </row>
     <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -2909,7 +2926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2923,10 +2940,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="46"/>
     </row>
     <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -3553,7 +3570,7 @@
       <c r="B81" s="13"/>
     </row>
   </sheetData>
-  <sortState ref="A4:B80">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B80">
     <sortCondition ref="B4"/>
   </sortState>
   <mergeCells count="1">
@@ -3567,7 +3584,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3581,10 +3598,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>301</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="46"/>
     </row>
     <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -3613,8 +3630,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3623,15 +3640,16 @@
     <col min="1" max="1" width="14.28515625" style="27" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>303</v>
       </c>
       <c r="B1" s="24"/>
     </row>
-    <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>304</v>
       </c>
@@ -3641,8 +3659,11 @@
       <c r="C3" s="5" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>307</v>
       </c>
@@ -3652,8 +3673,11 @@
       <c r="C4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>309</v>
       </c>
@@ -3663,8 +3687,11 @@
       <c r="C5" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>311</v>
       </c>
@@ -3674,8 +3701,11 @@
       <c r="C6" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
         <v>313</v>
       </c>
@@ -3685,8 +3715,11 @@
       <c r="C7" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>315</v>
       </c>
@@ -3696,8 +3729,11 @@
       <c r="C8" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
         <v>317</v>
       </c>
@@ -3706,6 +3742,9 @@
       </c>
       <c r="C9" s="2">
         <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -3716,7 +3755,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3736,16 +3775,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -4398,26 +4437,26 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="49"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="51"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="52"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="48"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="49"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
@@ -4573,7 +4612,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4590,14 +4629,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
@@ -4745,22 +4784,22 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="53"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
     </row>
     <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
@@ -4924,7 +4963,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4941,14 +4980,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
@@ -5227,23 +5266,23 @@
       <c r="G15" s="13"/>
     </row>
     <row r="16" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="56"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="58"/>
       <c r="G16" s="13"/>
     </row>
     <row r="17" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="55"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -5578,7 +5617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5593,12 +5632,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
@@ -5689,18 +5728,18 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="58"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="60"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="61"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="63"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="64"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -5730,7 +5769,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5745,12 +5784,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
@@ -6110,21 +6149,21 @@
       <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="58"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="60"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="61"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="61" t="s">
+      <c r="A26" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="63"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="64"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -6337,7 +6376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6352,12 +6391,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
@@ -7514,12 +7553,12 @@
       <c r="D80" s="28"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="64" t="s">
+      <c r="A81" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="B81" s="64"/>
-      <c r="C81" s="64"/>
-      <c r="D81" s="64"/>
+      <c r="B81" s="65"/>
+      <c r="C81" s="65"/>
+      <c r="D81" s="65"/>
       <c r="E81" s="13"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -7580,7 +7619,7 @@
       <c r="E88" s="13"/>
     </row>
   </sheetData>
-  <sortState ref="A4:D79">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D79">
     <sortCondition ref="B4"/>
   </sortState>
   <mergeCells count="2">
@@ -7595,7 +7634,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7611,13 +7650,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
@@ -7727,21 +7766,21 @@
       <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="65"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="67"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68"/>
       <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="70"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="71"/>
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>